<commit_message>
Fixed for exception on tripfolderpage and added fun for setting car price filter
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Mystifly.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Air/Air_Mystifly.xlsx
@@ -117,7 +117,7 @@
     <t>MYSTIFLY air oneway booking for INTERNATIONAL location for 1 adult .1 child and 1 infant with OnAccount payment mode.</t>
   </si>
   <si>
-    <t>25</t>
+    <t>25|40|50</t>
   </si>
 </sst>
 </file>
@@ -669,6 +669,36 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -1347,36 +1377,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
-          <color theme="4"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4"/>
-          <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <right style="thin">
           <color indexed="64"/>
         </right>
@@ -1415,23 +1415,23 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:Q5" totalsRowShown="0" headerRowDxfId="55" headerRowBorderDxfId="54" tableBorderDxfId="53">
   <autoFilter ref="A1:Q5"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="50"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="49"/>
-    <tableColumn id="3" name="TripType" dataDxfId="48"/>
-    <tableColumn id="4" name="AirPortPairs" dataDxfId="47"/>
-    <tableColumn id="5" name="TravelDates" dataDxfId="46"/>
-    <tableColumn id="6" name="Adults" dataDxfId="45"/>
-    <tableColumn id="7" name="Infants" dataDxfId="44"/>
-    <tableColumn id="8" name="Children" dataDxfId="43"/>
-    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="42"/>
-    <tableColumn id="10" name="CabinType" dataDxfId="41"/>
-    <tableColumn id="11" name="NonStopFlight" dataDxfId="40"/>
-    <tableColumn id="12" name="AirLines" dataDxfId="39"/>
-    <tableColumn id="13" name="PaymentMode" dataDxfId="38"/>
-    <tableColumn id="14" name="Supplier" dataDxfId="37"/>
-    <tableColumn id="15" name="UserType" dataDxfId="36"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="35"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="34"/>
+    <tableColumn id="1" name="Description" dataDxfId="52"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="51"/>
+    <tableColumn id="3" name="TripType" dataDxfId="50"/>
+    <tableColumn id="4" name="AirPortPairs" dataDxfId="49"/>
+    <tableColumn id="5" name="TravelDates" dataDxfId="48"/>
+    <tableColumn id="6" name="Adults" dataDxfId="47"/>
+    <tableColumn id="7" name="Infants" dataDxfId="46"/>
+    <tableColumn id="8" name="Children" dataDxfId="45"/>
+    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="44"/>
+    <tableColumn id="10" name="CabinType" dataDxfId="43"/>
+    <tableColumn id="11" name="NonStopFlight" dataDxfId="42"/>
+    <tableColumn id="12" name="AirLines" dataDxfId="41"/>
+    <tableColumn id="13" name="PaymentMode" dataDxfId="40"/>
+    <tableColumn id="14" name="Supplier" dataDxfId="39"/>
+    <tableColumn id="15" name="UserType" dataDxfId="38"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="37"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1441,30 +1441,30 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:Q2" totalsRowShown="0">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
-    <tableColumn id="1" name="Description" dataDxfId="33"/>
-    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="32"/>
-    <tableColumn id="3" name="TripType" dataDxfId="31"/>
-    <tableColumn id="4" name="AirPortPairs" dataDxfId="30"/>
-    <tableColumn id="5" name="TravelDates" dataDxfId="29"/>
-    <tableColumn id="6" name="Adults" dataDxfId="28"/>
-    <tableColumn id="7" name="Infants" dataDxfId="27"/>
-    <tableColumn id="8" name="Children" dataDxfId="26"/>
-    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="25"/>
-    <tableColumn id="10" name="CabinType" dataDxfId="24"/>
-    <tableColumn id="11" name="NonStopFlight" dataDxfId="23"/>
-    <tableColumn id="12" name="AirLines" dataDxfId="22"/>
-    <tableColumn id="13" name="PaymentMode" dataDxfId="21"/>
-    <tableColumn id="14" name="Supplier" dataDxfId="20"/>
-    <tableColumn id="15" name="UserType" dataDxfId="19"/>
-    <tableColumn id="16" name="PostFilters" dataDxfId="18"/>
-    <tableColumn id="17" name="PostFiltersValues" dataDxfId="17"/>
+    <tableColumn id="1" name="Description" dataDxfId="35"/>
+    <tableColumn id="2" name="ExecutionPipeline" dataDxfId="34"/>
+    <tableColumn id="3" name="TripType" dataDxfId="33"/>
+    <tableColumn id="4" name="AirPortPairs" dataDxfId="32"/>
+    <tableColumn id="5" name="TravelDates" dataDxfId="31"/>
+    <tableColumn id="6" name="Adults" dataDxfId="30"/>
+    <tableColumn id="7" name="Infants" dataDxfId="29"/>
+    <tableColumn id="8" name="Children" dataDxfId="28"/>
+    <tableColumn id="9" name="IncludeNearByAirPorts" dataDxfId="27"/>
+    <tableColumn id="10" name="CabinType" dataDxfId="26"/>
+    <tableColumn id="11" name="NonStopFlight" dataDxfId="25"/>
+    <tableColumn id="12" name="AirLines" dataDxfId="24"/>
+    <tableColumn id="13" name="PaymentMode" dataDxfId="23"/>
+    <tableColumn id="14" name="Supplier" dataDxfId="22"/>
+    <tableColumn id="15" name="UserType" dataDxfId="21"/>
+    <tableColumn id="16" name="PostFilters" dataDxfId="20"/>
+    <tableColumn id="17" name="PostFiltersValues" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="52" tableBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:Q2" totalsRowShown="0" headerRowDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="A1:Q2"/>
   <tableColumns count="17">
     <tableColumn id="1" name="Description" dataDxfId="16"/>
@@ -2190,7 +2190,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>